<commit_message>
feat: add TeamMembers API for managers to view reporting employees
</commit_message>
<xml_diff>
--- a/leave_management_doc.xlsx
+++ b/leave_management_doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29622"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://victopialabs-my.sharepoint.com/personal/lokesh_victopialabs_com/Documents/Desktop/Leave Management API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="11_F25DC773A252ABDACC10485E215959785BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFAA43C7-8DC9-406E-9BF7-8952A3CBD9B2}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_F25DC773A252ABDACC10485E215959785BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B52ACDE9-30C5-4396-B7DD-315A05C2FDF8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
feat: add API for admin to view the leave request by employees
</commit_message>
<xml_diff>
--- a/leave_management_doc.xlsx
+++ b/leave_management_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://victopialabs-my.sharepoint.com/personal/lokesh_victopialabs_com/Documents/Desktop/Leave Management API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_F25DC773A252ABDACC10485E215959785BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B52ACDE9-30C5-4396-B7DD-315A05C2FDF8}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_F25DC773A252ABDACC10485E215959785BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08DB2F47-BBA8-4B9C-AB08-B4405190FA76}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,16 +454,16 @@
     <t xml:space="preserve">  LeaveBalance                    </t>
   </si>
   <si>
-    <t>/api/admin/leave-balances/</t>
-  </si>
-  <si>
-    <t>Assign initial leave balances</t>
-  </si>
-  <si>
-    <t>{ user_id, CL, SL, PL }</t>
-  </si>
-  <si>
-    <t>{ balance_details }</t>
+    <t>/api/admin/leave-balances/{id}</t>
+  </si>
+  <si>
+    <t>Updating leave balances</t>
+  </si>
+  <si>
+    <t>{used_leaves}</t>
+  </si>
+  <si>
+    <t>{ total_leaves, used_leaves,remaining_leave}</t>
   </si>
   <si>
     <t>/api/admin/leaves/</t>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1827,7 +1827,7 @@
         <v>136</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="F92" s="4" t="s">
         <v>137</v>

</xml_diff>